<commit_message>
Temporary commit with recent changes for chart generation and dashboard
</commit_message>
<xml_diff>
--- a/Datasets/custom.xlsx
+++ b/Datasets/custom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waqar\Documents\Github Projects\Automatic-Data-Analytics-with-NLP\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2A25E5-0EDF-45D0-AFF9-C54358CAFC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EE1A78-D459-4E81-A49D-64E39964B249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17055" yWindow="16080" windowWidth="20730" windowHeight="11040" xr2:uid="{C0D43AE4-8ED8-4A5B-81D7-9C972FE35537}"/>
+    <workbookView xWindow="18615" yWindow="17640" windowWidth="15375" windowHeight="7785" xr2:uid="{C0D43AE4-8ED8-4A5B-81D7-9C972FE35537}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -485,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E5C9E5C-FE91-45EC-8CA4-78A28B3C685F}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,7 +567,7 @@
       <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="2">
         <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -613,14 +613,14 @@
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
+      <c r="C6" s="2">
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
+      <c r="E6" s="2">
+        <v>45678</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>18</v>
@@ -682,8 +682,8 @@
       <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>10</v>
+      <c r="C9" s="2">
+        <v>74</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
@@ -734,8 +734,8 @@
       <c r="D11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>10</v>
+      <c r="E11" s="2">
+        <v>845</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Now summary of uploaded dataset is being displayed on the preview.html page. Limited the prompt message for 20 words
</commit_message>
<xml_diff>
--- a/Datasets/custom.xlsx
+++ b/Datasets/custom.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Waqar\Documents\Github Projects\Automatic-Data-Analytics-with-NLP\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F05BFDC-CBBF-4D07-9448-9636369C14C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C85F86A-FE82-491B-A256-C87058BA6925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18615" yWindow="17640" windowWidth="15375" windowHeight="7785" xr2:uid="{C0D43AE4-8ED8-4A5B-81D7-9C972FE35537}"/>
+    <workbookView xWindow="17190" yWindow="16200" windowWidth="20460" windowHeight="10545" xr2:uid="{C0D43AE4-8ED8-4A5B-81D7-9C972FE35537}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -435,15 +438,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E5C9E5C-FE91-45EC-8CA4-78A28B3C685F}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D8"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,11 +459,8 @@
       <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -473,11 +473,8 @@
       <c r="D2" s="2">
         <v>3.5</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -490,28 +487,22 @@
       <c r="D3" s="2">
         <v>1.2</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2">
-        <v>2</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -524,11 +515,8 @@
       <c r="D5" s="2">
         <v>2.8</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -541,28 +529,22 @@
       <c r="D6" s="2">
         <v>4</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D7" s="2">
-        <v>5.5</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -575,38 +557,27 @@
       <c r="D8" s="2">
         <v>3</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>